<commit_message>
Replace preserveBackslash option by escape option & add ad hoc test
</commit_message>
<xml_diff>
--- a/test/acceptance/data/xlsx-test/from_xlsx_input.xlsx
+++ b/test/acceptance/data/xlsx-test/from_xlsx_input.xlsx
@@ -56,10 +56,10 @@
     <t>xlsx.v4</t>
   </si>
   <si>
-    <t>xlsx.v2</t>
-  </si>
-  <si>
     <t>xlsx.v1</t>
+  </si>
+  <si>
+    <t>xlsx.v2\n</t>
   </si>
 </sst>
 </file>
@@ -535,7 +535,7 @@
   <dimension ref="B2:D11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F10" sqref="F10"/>
+      <selection activeCell="G7" sqref="G7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -560,7 +560,7 @@
       </c>
       <c r="C4" s="4"/>
       <c r="D4" s="5" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="5" spans="2:4" x14ac:dyDescent="0.2">
@@ -569,7 +569,7 @@
       </c>
       <c r="C5" s="1"/>
       <c r="D5" s="7" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="6" spans="2:4" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
Last line automatic detection
</commit_message>
<xml_diff>
--- a/test/acceptance/data/xlsx-test/from_xlsx_input.xlsx
+++ b/test/acceptance/data/xlsx-test/from_xlsx_input.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="1440" yWindow="1860" windowWidth="27360" windowHeight="15320" tabRatio="500"/>
+    <workbookView xWindow="1440" yWindow="1840" windowWidth="27360" windowHeight="15320" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -101,7 +101,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="11">
+  <borders count="8">
     <border>
       <left/>
       <right/>
@@ -212,56 +212,11 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="medium">
-        <color auto="1"/>
-      </left>
-      <right style="thin">
-        <color auto="1"/>
-      </right>
-      <top style="thin">
-        <color auto="1"/>
-      </top>
-      <bottom style="medium">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color auto="1"/>
-      </left>
-      <right style="thin">
-        <color auto="1"/>
-      </right>
-      <top style="thin">
-        <color auto="1"/>
-      </top>
-      <bottom style="medium">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color auto="1"/>
-      </left>
-      <right style="medium">
-        <color auto="1"/>
-      </right>
-      <top style="thin">
-        <color auto="1"/>
-      </top>
-      <bottom style="medium">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
@@ -270,9 +225,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -550,10 +502,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:D13"/>
+  <dimension ref="B2:D14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F8" sqref="F8"/>
+      <selection activeCell="E21" sqref="E21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -642,25 +594,30 @@
       </c>
     </row>
     <row r="11" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B11" s="6" t="s">
-        <v>6</v>
-      </c>
-      <c r="C11" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="D11" s="7" t="s">
-        <v>7</v>
-      </c>
+      <c r="B11" s="6"/>
+      <c r="C11" s="1"/>
+      <c r="D11" s="7"/>
     </row>
     <row r="12" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B12" s="6"/>
       <c r="C12" s="1"/>
       <c r="D12" s="7"/>
     </row>
-    <row r="13" spans="2:4" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B13" s="8"/>
-      <c r="C13" s="9"/>
-      <c r="D13" s="10"/>
+    <row r="13" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B13" s="6"/>
+      <c r="C13" s="1"/>
+      <c r="D13" s="7"/>
+    </row>
+    <row r="14" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B14" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D14" s="7" t="s">
+        <v>7</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>